<commit_message>
Model def file structure updates.
</commit_message>
<xml_diff>
--- a/models/test_structures/piecewise_test.xlsx
+++ b/models/test_structures/piecewise_test.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufr/code/sifra/models/test_structures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{625E5D5A-F8CB-1947-8DA6-5C03E5FDDE04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28695" windowHeight="16845" tabRatio="804" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="16840" tabRatio="804" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="11" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <sheet name="comp_type_dmg_algo" sheetId="9" r:id="rId6"/>
     <sheet name="damage_state_def" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="119">
   <si>
     <t>component_type</t>
   </si>
@@ -374,18 +380,27 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>recovery_function</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2270,19 +2285,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -2293,7 +2308,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -2304,7 +2319,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -2315,7 +2330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -2326,7 +2341,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -2337,7 +2352,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -2348,7 +2363,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -2362,8 +2377,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <tabColor rgb="FF66CCFF"/>
   </sheetPr>
   <dimension ref="A1:G13"/>
@@ -2372,9 +2387,9 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="3" width="30.625" style="40" customWidth="1"/>
+    <col min="1" max="3" width="30.6640625" style="40" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="40" customWidth="1"/>
     <col min="5" max="5" width="19" style="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" style="40" customWidth="1"/>
@@ -2382,7 +2397,7 @@
     <col min="8" max="16384" width="11" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="37" t="s">
         <v>40</v>
       </c>
@@ -2405,7 +2420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="17" customHeight="1">
       <c r="A2" s="40" t="s">
         <v>70</v>
       </c>
@@ -2428,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="17" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>80</v>
       </c>
@@ -2451,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="17" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>81</v>
       </c>
@@ -2474,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>82</v>
       </c>
@@ -2497,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>83</v>
       </c>
@@ -2520,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17" customHeight="1">
       <c r="A7" s="27" t="s">
         <v>13</v>
       </c>
@@ -2543,27 +2558,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="D8" s="44"/>
       <c r="G8" s="44"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="D9" s="44"/>
       <c r="G9" s="44"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="D10" s="44"/>
       <c r="G10" s="44"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="D11" s="44"/>
       <c r="G11" s="44"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="D12" s="45"/>
       <c r="G12" s="45"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="D13" s="45"/>
       <c r="G13" s="45"/>
     </row>
@@ -2574,8 +2589,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <tabColor rgb="FF66CCFF"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
@@ -2584,15 +2599,15 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19" style="27" customWidth="1"/>
     <col min="2" max="2" width="18" style="27" customWidth="1"/>
-    <col min="3" max="4" width="13.375" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="27"/>
+    <col min="3" max="4" width="13.33203125" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26" customHeight="1">
       <c r="A1" s="37" t="s">
         <v>57</v>
       </c>
@@ -2606,7 +2621,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>70</v>
       </c>
@@ -2620,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>80</v>
       </c>
@@ -2634,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>81</v>
       </c>
@@ -2648,7 +2663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>83</v>
       </c>
@@ -2662,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="20" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>82</v>
       </c>
@@ -2676,22 +2691,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="20" customHeight="1">
       <c r="C7" s="47"/>
     </row>
-    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="20" customHeight="1">
       <c r="C8" s="47"/>
     </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="C9" s="47"/>
     </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="C10" s="47"/>
     </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="C11" s="47"/>
     </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="C12" s="47"/>
     </row>
   </sheetData>
@@ -2701,8 +2716,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <tabColor rgb="FF80FF00"/>
   </sheetPr>
   <dimension ref="A1:D9"/>
@@ -2711,16 +2726,16 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="17.875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="27" customWidth="1"/>
     <col min="4" max="4" width="18" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="27"/>
+    <col min="5" max="16384" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26" customHeight="1">
       <c r="A1" s="28" t="s">
         <v>60</v>
       </c>
@@ -2734,7 +2749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>70</v>
       </c>
@@ -2748,29 +2763,29 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="33"/>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
       <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
     </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="C5" s="34"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="C6" s="34"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="C8" s="34"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="C9" s="34"/>
     </row>
   </sheetData>
@@ -2780,8 +2795,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
     <tabColor rgb="FF80FF00"/>
   </sheetPr>
   <dimension ref="A1:F3"/>
@@ -2790,16 +2805,16 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="22" style="27" customWidth="1"/>
-    <col min="3" max="3" width="21.625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="11.375" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="27"/>
+    <col min="3" max="3" width="21.6640625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="27" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26" customHeight="1">
       <c r="A1" s="28" t="s">
         <v>63</v>
       </c>
@@ -2816,7 +2831,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>13</v>
       </c>
@@ -2834,7 +2849,7 @@
       </c>
       <c r="F2" s="34"/>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="33"/>
       <c r="C3" s="36"/>
       <c r="D3" s="31"/>
@@ -2847,37 +2862,38 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
     <tabColor rgb="FF804000"/>
   </sheetPr>
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="88"/>
-    <col min="2" max="2" width="22.625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="88"/>
+    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="8" width="14.125" style="2" customWidth="1"/>
-    <col min="9" max="13" width="11.125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="12.625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="65.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="44.625" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="10.875" style="3"/>
+    <col min="7" max="9" width="14.1640625" style="2" customWidth="1"/>
+    <col min="10" max="14" width="11.1640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.5" style="2" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="65.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="44.6640625" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="26" customHeight="1">
       <c r="A1" s="88" t="s">
         <v>108</v>
       </c>
@@ -2900,37 +2916,43 @@
         <v>107</v>
       </c>
       <c r="H1" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="L1" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="M1" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="N1" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="56" t="s">
+      <c r="O1" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="56" t="s">
+      <c r="Q1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="56" t="s">
+      <c r="R1" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="77" t="s">
+      <c r="S1" s="77" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="15" customFormat="1">
       <c r="A2" s="89">
         <v>1</v>
       </c>
@@ -2953,38 +2975,44 @@
         <v>2</v>
       </c>
       <c r="H2" s="19">
+        <v>0</v>
+      </c>
+      <c r="I2" s="19">
         <v>0.375</v>
       </c>
-      <c r="I2" s="20">
+      <c r="J2" s="20">
         <v>0.1</v>
       </c>
-      <c r="J2" s="20">
-        <v>1</v>
-      </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="20">
+        <v>1</v>
+      </c>
+      <c r="L2" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="52">
+      <c r="M2" s="52">
         <v>10</v>
       </c>
-      <c r="M2" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="4">
-        <v>1</v>
-      </c>
-      <c r="O2" s="20">
-        <f t="shared" ref="O2" si="0">P2/NORMINV(0.95,0,1)</f>
+      <c r="N2" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="20">
+        <f t="shared" ref="Q2" si="0">R2/NORMINV(0.95,0,1)</f>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P2" s="78">
+      <c r="R2" s="78">
         <v>0.5</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="15" customFormat="1">
       <c r="A3" s="89">
         <v>2</v>
       </c>
@@ -3007,38 +3035,44 @@
         <v>2</v>
       </c>
       <c r="H3" s="19">
+        <v>0</v>
+      </c>
+      <c r="I3" s="19">
         <v>0.375</v>
       </c>
-      <c r="I3" s="20">
+      <c r="J3" s="20">
         <v>0.1</v>
       </c>
-      <c r="J3" s="20">
-        <v>1</v>
-      </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="20">
+        <v>1</v>
+      </c>
+      <c r="L3" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="52">
+      <c r="M3" s="52">
         <v>20</v>
       </c>
-      <c r="M3" s="52">
+      <c r="N3" s="52">
         <v>10</v>
       </c>
-      <c r="N3" s="4">
-        <v>1</v>
-      </c>
-      <c r="O3" s="20">
-        <f t="shared" ref="O3:O4" si="1">P3/NORMINV(0.95,0,1)</f>
+      <c r="O3" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="20">
+        <f t="shared" ref="Q3:Q4" si="1">R3/NORMINV(0.95,0,1)</f>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P3" s="78">
+      <c r="R3" s="78">
         <v>0.5</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="15" customFormat="1">
       <c r="A4" s="89">
         <v>3</v>
       </c>
@@ -3061,38 +3095,44 @@
         <v>2</v>
       </c>
       <c r="H4" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
         <v>0.375</v>
       </c>
-      <c r="I4" s="20">
+      <c r="J4" s="20">
         <v>0.1</v>
       </c>
-      <c r="J4" s="20">
-        <v>1</v>
-      </c>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="20">
+        <v>1</v>
+      </c>
+      <c r="L4" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="52">
+      <c r="M4" s="52">
         <v>30</v>
       </c>
-      <c r="M4" s="52">
+      <c r="N4" s="52">
         <v>20</v>
       </c>
-      <c r="N4" s="4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="20">
+      <c r="O4" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="20">
         <f t="shared" si="1"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P4" s="78">
+      <c r="R4" s="78">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="15" customFormat="1">
       <c r="A5" s="89">
         <v>4</v>
       </c>
@@ -3115,38 +3155,44 @@
         <v>2</v>
       </c>
       <c r="H5" s="19">
+        <v>0</v>
+      </c>
+      <c r="I5" s="19">
         <v>0.375</v>
       </c>
-      <c r="I5" s="20">
+      <c r="J5" s="20">
         <v>0.1</v>
       </c>
-      <c r="J5" s="20">
-        <v>1</v>
-      </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="20">
+        <v>1</v>
+      </c>
+      <c r="L5" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M5" s="52">
+      <c r="M5" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="N5" s="52">
         <v>30</v>
       </c>
-      <c r="N5" s="4">
-        <v>1</v>
-      </c>
-      <c r="O5" s="20">
-        <f t="shared" ref="O5:O20" si="2">P5/NORMINV(0.95,0,1)</f>
+      <c r="O5" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="20">
+        <f t="shared" ref="Q5:Q20" si="2">R5/NORMINV(0.95,0,1)</f>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P5" s="78">
+      <c r="R5" s="78">
         <v>0.5</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="15" customFormat="1">
       <c r="A6" s="89">
         <v>5</v>
       </c>
@@ -3156,7 +3202,7 @@
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -3169,38 +3215,44 @@
         <v>0.57000000000000006</v>
       </c>
       <c r="H6" s="21">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
         <v>0.375</v>
       </c>
-      <c r="I6" s="22">
+      <c r="J6" s="22">
         <v>0.3</v>
       </c>
-      <c r="J6" s="22">
+      <c r="K6" s="22">
         <v>0</v>
       </c>
-      <c r="K6" s="53" t="s">
+      <c r="L6" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L6" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M6" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N6" s="6">
+      <c r="M6" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N6" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O6" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" s="6">
         <v>3</v>
       </c>
-      <c r="O6" s="22">
+      <c r="Q6" s="22">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P6" s="79">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="12" t="s">
+      <c r="R6" s="79">
+        <v>1</v>
+      </c>
+      <c r="S6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="15" customFormat="1">
       <c r="A7" s="89">
         <v>6</v>
       </c>
@@ -3210,7 +3262,7 @@
       <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -3223,38 +3275,44 @@
         <v>0.78</v>
       </c>
       <c r="H7" s="21">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
         <v>0.47499999999999998</v>
       </c>
-      <c r="I7" s="22">
+      <c r="J7" s="22">
         <v>0.75</v>
       </c>
-      <c r="J7" s="22">
+      <c r="K7" s="22">
         <v>0</v>
       </c>
-      <c r="K7" s="53" t="s">
+      <c r="L7" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M7" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N7" s="6">
+      <c r="M7" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O7" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P7" s="6">
         <v>15</v>
       </c>
-      <c r="O7" s="22">
+      <c r="Q7" s="22">
         <f t="shared" si="2"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="P7" s="79">
+      <c r="R7" s="79">
         <v>3</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="15" customFormat="1">
       <c r="A8" s="89">
         <v>7</v>
       </c>
@@ -3264,7 +3322,7 @@
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -3277,38 +3335,44 @@
         <v>1.33</v>
       </c>
       <c r="H8" s="21">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21">
         <v>0.47499999999999998</v>
       </c>
-      <c r="I8" s="22">
-        <v>1</v>
-      </c>
       <c r="J8" s="22">
+        <v>1</v>
+      </c>
+      <c r="K8" s="22">
         <v>0</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="L8" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M8" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N8" s="6">
+      <c r="M8" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N8" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P8" s="6">
         <v>30</v>
       </c>
-      <c r="O8" s="22">
+      <c r="Q8" s="22">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P8" s="79">
+      <c r="R8" s="79">
         <v>4</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="S8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="15" customFormat="1">
       <c r="A9" s="89">
         <v>8</v>
       </c>
@@ -3331,38 +3395,44 @@
         <v>0.35</v>
       </c>
       <c r="H9" s="19">
+        <v>0</v>
+      </c>
+      <c r="I9" s="19">
         <v>0.4</v>
       </c>
-      <c r="I9" s="20">
+      <c r="J9" s="20">
         <v>0.1</v>
       </c>
-      <c r="J9" s="23">
+      <c r="K9" s="23">
         <v>0</v>
       </c>
-      <c r="K9" s="52" t="s">
+      <c r="L9" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="52" t="s">
-        <v>113</v>
-      </c>
       <c r="M9" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="O9" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P9" s="4">
         <v>5</v>
       </c>
-      <c r="O9" s="20">
+      <c r="Q9" s="20">
         <f t="shared" si="2"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P9" s="78">
+      <c r="R9" s="78">
         <v>0.5</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="S9" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="15" customFormat="1">
       <c r="A10" s="89">
         <v>9</v>
       </c>
@@ -3372,7 +3442,7 @@
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -3385,38 +3455,44 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="H10" s="21">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
         <v>0.5</v>
       </c>
-      <c r="I10" s="22">
+      <c r="J10" s="22">
         <v>0.3</v>
       </c>
-      <c r="J10" s="22">
+      <c r="K10" s="22">
         <v>0</v>
       </c>
-      <c r="K10" s="53" t="s">
+      <c r="L10" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M10" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N10" s="6">
+      <c r="M10" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N10" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O10" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P10" s="6">
         <v>17</v>
       </c>
-      <c r="O10" s="22">
+      <c r="Q10" s="22">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P10" s="79">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="12" t="s">
+      <c r="R10" s="79">
+        <v>1</v>
+      </c>
+      <c r="S10" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="15" customFormat="1">
       <c r="A11" s="89">
         <v>10</v>
       </c>
@@ -3426,7 +3502,7 @@
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -3439,38 +3515,44 @@
         <v>0.75</v>
       </c>
       <c r="H11" s="21">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
         <v>0.4</v>
       </c>
-      <c r="I11" s="22">
+      <c r="J11" s="22">
         <v>0.75</v>
       </c>
-      <c r="J11" s="22">
+      <c r="K11" s="22">
         <v>0</v>
       </c>
-      <c r="K11" s="53" t="s">
+      <c r="L11" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M11" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N11" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O11" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P11" s="6">
         <v>37</v>
       </c>
-      <c r="O11" s="22">
+      <c r="Q11" s="22">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P11" s="79">
+      <c r="R11" s="79">
         <v>2</v>
       </c>
-      <c r="Q11" s="12" t="s">
+      <c r="S11" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="15" customFormat="1">
       <c r="A12" s="89">
         <v>11</v>
       </c>
@@ -3480,7 +3562,7 @@
       <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -3493,39 +3575,45 @@
         <v>1</v>
       </c>
       <c r="H12" s="21">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21">
         <v>0.4</v>
       </c>
-      <c r="I12" s="22">
-        <v>1</v>
-      </c>
       <c r="J12" s="22">
+        <v>1</v>
+      </c>
+      <c r="K12" s="22">
         <v>0</v>
       </c>
-      <c r="K12" s="53" t="s">
+      <c r="L12" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M12" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N12" s="17">
+      <c r="M12" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N12" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O12" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P12" s="17">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O12" s="22">
+      <c r="Q12" s="22">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P12" s="79">
+      <c r="R12" s="79">
         <v>4</v>
       </c>
-      <c r="Q12" s="12" t="s">
+      <c r="S12" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="15" customFormat="1">
       <c r="A13" s="89">
         <v>12</v>
       </c>
@@ -3548,38 +3636,44 @@
         <v>0.75</v>
       </c>
       <c r="H13" s="19">
+        <v>0</v>
+      </c>
+      <c r="I13" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I13" s="20">
+      <c r="J13" s="20">
         <v>0.03</v>
       </c>
-      <c r="J13" s="23">
+      <c r="K13" s="23">
         <v>0</v>
       </c>
-      <c r="K13" s="52" t="s">
+      <c r="L13" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="52" t="s">
-        <v>113</v>
-      </c>
       <c r="M13" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="O13" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P13" s="4">
         <v>3</v>
       </c>
-      <c r="O13" s="20">
+      <c r="Q13" s="20">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P13" s="78">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="11" t="s">
+      <c r="R13" s="78">
+        <v>1</v>
+      </c>
+      <c r="S13" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="15" customFormat="1">
       <c r="A14" s="89">
         <v>13</v>
       </c>
@@ -3589,7 +3683,7 @@
       <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -3602,38 +3696,44 @@
         <v>1</v>
       </c>
       <c r="H14" s="21">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
         <v>0.3</v>
       </c>
-      <c r="I14" s="22">
+      <c r="J14" s="22">
         <v>0.15</v>
       </c>
-      <c r="J14" s="22">
+      <c r="K14" s="22">
         <v>0</v>
       </c>
-      <c r="K14" s="53" t="s">
+      <c r="L14" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L14" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M14" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N14" s="6">
+      <c r="M14" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N14" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O14" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="6">
         <v>20</v>
       </c>
-      <c r="O14" s="22">
+      <c r="Q14" s="22">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P14" s="79">
+      <c r="R14" s="79">
         <v>2</v>
       </c>
-      <c r="Q14" s="12" t="s">
+      <c r="S14" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="15" customFormat="1">
       <c r="A15" s="89">
         <v>14</v>
       </c>
@@ -3643,7 +3743,7 @@
       <c r="C15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -3656,38 +3756,44 @@
         <v>1.33</v>
       </c>
       <c r="H15" s="21">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21">
         <v>0.34</v>
       </c>
-      <c r="I15" s="22">
+      <c r="J15" s="22">
         <v>0.4</v>
       </c>
-      <c r="J15" s="22">
+      <c r="K15" s="22">
         <v>0</v>
       </c>
-      <c r="K15" s="53" t="s">
+      <c r="L15" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L15" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M15" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="M15" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N15" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O15" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P15" s="6">
         <v>60</v>
       </c>
-      <c r="O15" s="22">
+      <c r="Q15" s="22">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P15" s="79">
+      <c r="R15" s="79">
         <v>4</v>
       </c>
-      <c r="Q15" s="12" t="s">
+      <c r="S15" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="15" customFormat="1">
       <c r="A16" s="89">
         <v>15</v>
       </c>
@@ -3697,7 +3803,7 @@
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -3710,39 +3816,45 @@
         <v>1.55</v>
       </c>
       <c r="H16" s="21">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I16" s="22">
+      <c r="J16" s="22">
         <v>1.2</v>
       </c>
-      <c r="J16" s="22">
+      <c r="K16" s="22">
         <v>0</v>
       </c>
-      <c r="K16" s="53" t="s">
+      <c r="L16" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M16" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N16" s="17">
+      <c r="M16" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N16" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O16" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P16" s="17">
         <f>24*30/7</f>
         <v>102.85714285714286</v>
       </c>
-      <c r="O16" s="22">
+      <c r="Q16" s="22">
         <f t="shared" si="2"/>
         <v>4.8636546552941553</v>
       </c>
-      <c r="P16" s="79">
+      <c r="R16" s="79">
         <v>8</v>
       </c>
-      <c r="Q16" s="12" t="s">
+      <c r="S16" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="15" customFormat="1">
       <c r="A17" s="89">
         <v>16</v>
       </c>
@@ -3765,38 +3877,44 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H17" s="19">
+        <v>0</v>
+      </c>
+      <c r="I17" s="19">
         <v>0.25</v>
       </c>
-      <c r="I17" s="20">
+      <c r="J17" s="20">
         <v>0.05</v>
       </c>
-      <c r="J17" s="23">
-        <v>1</v>
-      </c>
-      <c r="K17" s="52" t="s">
+      <c r="K17" s="23">
+        <v>1</v>
+      </c>
+      <c r="L17" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="52" t="s">
-        <v>113</v>
-      </c>
       <c r="M17" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="N17" s="20">
-        <v>1</v>
-      </c>
-      <c r="O17" s="20">
+      <c r="N17" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="O17" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P17" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="20">
         <f t="shared" si="2"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P17" s="20">
+      <c r="R17" s="20">
         <v>0.5</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="S17" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="15" customFormat="1">
       <c r="A18" s="89">
         <v>17</v>
       </c>
@@ -3806,7 +3924,7 @@
       <c r="C18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -3819,38 +3937,44 @@
         <v>0.43</v>
       </c>
       <c r="H18" s="21">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
         <v>0.35</v>
       </c>
-      <c r="I18" s="22">
+      <c r="J18" s="22">
         <v>0.3</v>
       </c>
-      <c r="J18" s="22">
+      <c r="K18" s="22">
         <v>0</v>
       </c>
-      <c r="K18" s="53" t="s">
+      <c r="L18" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M18" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N18" s="22">
+      <c r="M18" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N18" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O18" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P18" s="22">
         <v>3</v>
       </c>
-      <c r="O18" s="22">
+      <c r="Q18" s="22">
         <f t="shared" si="2"/>
         <v>0.91193524786765412</v>
       </c>
-      <c r="P18" s="22">
+      <c r="R18" s="22">
         <v>1.5</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="S18" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="15" customFormat="1">
       <c r="A19" s="89">
         <v>18</v>
       </c>
@@ -3860,7 +3984,7 @@
       <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -3873,38 +3997,44 @@
         <v>0.6</v>
       </c>
       <c r="H19" s="21">
+        <v>0</v>
+      </c>
+      <c r="I19" s="21">
         <v>0.4</v>
       </c>
-      <c r="I19" s="22">
+      <c r="J19" s="22">
         <v>0.75</v>
       </c>
-      <c r="J19" s="22">
+      <c r="K19" s="22">
         <v>0</v>
       </c>
-      <c r="K19" s="53" t="s">
+      <c r="L19" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L19" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M19" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N19" s="22">
+      <c r="M19" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N19" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O19" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P19" s="22">
         <v>7</v>
       </c>
-      <c r="O19" s="22">
+      <c r="Q19" s="22">
         <f t="shared" si="2"/>
         <v>2.1278489116911929</v>
       </c>
-      <c r="P19" s="22">
+      <c r="R19" s="22">
         <v>3.5</v>
       </c>
-      <c r="Q19" s="11" t="s">
+      <c r="S19" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="15" customFormat="1">
       <c r="A20" s="89">
         <v>19</v>
       </c>
@@ -3914,7 +4044,7 @@
       <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -3927,38 +4057,44 @@
         <v>0.85</v>
       </c>
       <c r="H20" s="21">
+        <v>0</v>
+      </c>
+      <c r="I20" s="21">
         <v>0.4</v>
       </c>
-      <c r="I20" s="22">
-        <v>1</v>
-      </c>
       <c r="J20" s="22">
+        <v>1</v>
+      </c>
+      <c r="K20" s="22">
         <v>0</v>
       </c>
-      <c r="K20" s="53" t="s">
+      <c r="L20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M20" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N20" s="22">
+      <c r="M20" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N20" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O20" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P20" s="22">
         <v>30</v>
       </c>
-      <c r="O20" s="22">
+      <c r="Q20" s="22">
         <f t="shared" si="2"/>
         <v>9.1193524786765412</v>
       </c>
-      <c r="P20" s="22">
+      <c r="R20" s="22">
         <v>15</v>
       </c>
-      <c r="Q20" s="11" t="s">
+      <c r="S20" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="15" customFormat="1">
       <c r="A21" s="89">
         <v>20</v>
       </c>
@@ -3981,38 +4117,44 @@
         <v>0.47500000000000003</v>
       </c>
       <c r="H21" s="19">
+        <v>0</v>
+      </c>
+      <c r="I21" s="19">
         <v>0.25</v>
       </c>
-      <c r="I21" s="20">
+      <c r="J21" s="20">
         <v>0.06</v>
       </c>
-      <c r="J21" s="20">
-        <v>1</v>
-      </c>
-      <c r="K21" s="52" t="s">
+      <c r="K21" s="20">
+        <v>1</v>
+      </c>
+      <c r="L21" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="52" t="s">
-        <v>113</v>
-      </c>
       <c r="M21" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="N21" s="74">
+      <c r="N21" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P21" s="74">
         <v>5</v>
       </c>
-      <c r="O21" s="80">
-        <f t="shared" ref="O21:O24" si="3">P21/NORMINV(0.95,0,1)</f>
+      <c r="Q21" s="80">
+        <f t="shared" ref="Q21:Q24" si="3">R21/NORMINV(0.95,0,1)</f>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P21" s="81">
+      <c r="R21" s="81">
         <v>0.5</v>
       </c>
-      <c r="Q21" s="11" t="s">
+      <c r="S21" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="15" customFormat="1">
       <c r="A22" s="89">
         <v>21</v>
       </c>
@@ -4022,7 +4164,7 @@
       <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -4035,38 +4177,44 @@
         <v>0.61499999999999999</v>
       </c>
       <c r="H22" s="21">
+        <v>0</v>
+      </c>
+      <c r="I22" s="21">
         <v>0.33</v>
       </c>
-      <c r="I22" s="22">
+      <c r="J22" s="22">
         <v>0.3</v>
       </c>
-      <c r="J22" s="22">
-        <v>1</v>
-      </c>
-      <c r="K22" s="53" t="s">
+      <c r="K22" s="22">
+        <v>1</v>
+      </c>
+      <c r="L22" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L22" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M22" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N22" s="75">
+      <c r="M22" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N22" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O22" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P22" s="75">
         <v>17</v>
       </c>
-      <c r="O22" s="82">
+      <c r="Q22" s="82">
         <f t="shared" si="3"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P22" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="11" t="s">
+      <c r="R22" s="83">
+        <v>1</v>
+      </c>
+      <c r="S22" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="15" customFormat="1">
       <c r="A23" s="89">
         <v>22</v>
       </c>
@@ -4076,7 +4224,7 @@
       <c r="C23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -4089,38 +4237,44 @@
         <v>0.77</v>
       </c>
       <c r="H23" s="21">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21">
         <v>0.4</v>
       </c>
-      <c r="I23" s="22">
+      <c r="J23" s="22">
         <v>0.75</v>
       </c>
-      <c r="J23" s="22">
+      <c r="K23" s="22">
         <v>0</v>
       </c>
-      <c r="K23" s="53" t="s">
+      <c r="L23" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L23" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M23" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N23" s="75">
+      <c r="M23" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="N23" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="O23" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="P23" s="75">
         <v>37</v>
       </c>
-      <c r="O23" s="82">
+      <c r="Q23" s="82">
         <f t="shared" si="3"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P23" s="83">
+      <c r="R23" s="83">
         <v>2</v>
       </c>
-      <c r="Q23" s="11" t="s">
+      <c r="S23" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="15" customFormat="1">
       <c r="A24" s="89">
         <v>23</v>
       </c>
@@ -4130,7 +4284,7 @@
       <c r="C24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>110</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -4143,39 +4297,45 @@
         <v>1</v>
       </c>
       <c r="H24" s="24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="24">
         <v>0.4</v>
       </c>
-      <c r="I24" s="25">
-        <v>1</v>
-      </c>
       <c r="J24" s="25">
+        <v>1</v>
+      </c>
+      <c r="K24" s="25">
         <v>0</v>
       </c>
-      <c r="K24" s="54" t="s">
+      <c r="L24" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M24" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N24" s="76">
+      <c r="M24" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="N24" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="O24" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="P24" s="76">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O24" s="82">
+      <c r="Q24" s="82">
         <f t="shared" si="3"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P24" s="83">
+      <c r="R24" s="83">
         <v>4</v>
       </c>
-      <c r="Q24" s="11" t="s">
+      <c r="S24" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="15" customFormat="1">
       <c r="A25" s="89">
         <v>24</v>
       </c>
@@ -4185,7 +4345,7 @@
       <c r="C25" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="58" t="s">
         <v>110</v>
       </c>
       <c r="E25" s="58" t="s">
@@ -4198,38 +4358,44 @@
         <v>10</v>
       </c>
       <c r="H25" s="60">
+        <v>0</v>
+      </c>
+      <c r="I25" s="60">
         <v>0.01</v>
       </c>
-      <c r="I25" s="61">
+      <c r="J25" s="61">
         <v>0.01</v>
       </c>
-      <c r="J25" s="61">
-        <v>1</v>
-      </c>
-      <c r="K25" s="61" t="s">
+      <c r="K25" s="61">
+        <v>1</v>
+      </c>
+      <c r="L25" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M25" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N25" s="62">
-        <v>1</v>
-      </c>
-      <c r="O25" s="61">
-        <f t="shared" ref="O25:O32" si="4">P25/NORMINV(0.95,0,1)</f>
+      <c r="M25" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="N25" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="O25" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="P25" s="62">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="61">
+        <f t="shared" ref="Q25:Q32" si="4">R25/NORMINV(0.95,0,1)</f>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P25" s="84">
+      <c r="R25" s="84">
         <v>0.1</v>
       </c>
-      <c r="Q25" s="11" t="s">
+      <c r="S25" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" s="15" customFormat="1">
       <c r="A26" s="89">
         <v>25</v>
       </c>
@@ -4239,7 +4405,7 @@
       <c r="C26" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="63" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="63" t="s">
@@ -4252,38 +4418,44 @@
         <v>10</v>
       </c>
       <c r="H26" s="65">
+        <v>0</v>
+      </c>
+      <c r="I26" s="65">
         <v>0.01</v>
       </c>
-      <c r="I26" s="66">
+      <c r="J26" s="66">
         <v>0.01</v>
       </c>
-      <c r="J26" s="66">
-        <v>1</v>
-      </c>
-      <c r="K26" s="66" t="s">
+      <c r="K26" s="66">
+        <v>1</v>
+      </c>
+      <c r="L26" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M26" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N26" s="67">
-        <v>1</v>
-      </c>
-      <c r="O26" s="66">
+      <c r="M26" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="N26" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="O26" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="P26" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="66">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P26" s="85">
+      <c r="R26" s="85">
         <v>0.1</v>
       </c>
-      <c r="Q26" s="11" t="s">
+      <c r="S26" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="15" customFormat="1">
       <c r="A27" s="89">
         <v>26</v>
       </c>
@@ -4293,7 +4465,7 @@
       <c r="C27" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="63" t="s">
         <v>110</v>
       </c>
       <c r="E27" s="63" t="s">
@@ -4306,38 +4478,44 @@
         <v>10</v>
       </c>
       <c r="H27" s="65">
+        <v>0</v>
+      </c>
+      <c r="I27" s="65">
         <v>0.01</v>
       </c>
-      <c r="I27" s="66">
+      <c r="J27" s="66">
         <v>0.01</v>
       </c>
-      <c r="J27" s="66">
-        <v>1</v>
-      </c>
-      <c r="K27" s="66" t="s">
+      <c r="K27" s="66">
+        <v>1</v>
+      </c>
+      <c r="L27" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M27" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N27" s="67">
-        <v>1</v>
-      </c>
-      <c r="O27" s="66">
+      <c r="M27" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="N27" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="O27" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="P27" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="66">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P27" s="85">
+      <c r="R27" s="85">
         <v>0.1</v>
       </c>
-      <c r="Q27" s="11" t="s">
+      <c r="S27" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="15" customFormat="1">
       <c r="A28" s="89">
         <v>27</v>
       </c>
@@ -4347,7 +4525,7 @@
       <c r="C28" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="68" t="s">
         <v>110</v>
       </c>
       <c r="E28" s="68" t="s">
@@ -4360,38 +4538,44 @@
         <v>10</v>
       </c>
       <c r="H28" s="70">
+        <v>0</v>
+      </c>
+      <c r="I28" s="70">
         <v>0.01</v>
       </c>
-      <c r="I28" s="71">
+      <c r="J28" s="71">
         <v>0.01</v>
       </c>
-      <c r="J28" s="71">
-        <v>1</v>
-      </c>
-      <c r="K28" s="71" t="s">
+      <c r="K28" s="71">
+        <v>1</v>
+      </c>
+      <c r="L28" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="L28" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M28" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N28" s="72">
-        <v>1</v>
-      </c>
-      <c r="O28" s="71">
+      <c r="M28" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="N28" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="O28" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="P28" s="72">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="71">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P28" s="86">
+      <c r="R28" s="86">
         <v>0.1</v>
       </c>
-      <c r="Q28" s="11" t="s">
+      <c r="S28" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="15" customFormat="1">
       <c r="A29" s="89">
         <v>28</v>
       </c>
@@ -4401,7 +4585,7 @@
       <c r="C29" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="58" t="s">
         <v>110</v>
       </c>
       <c r="E29" s="58" t="s">
@@ -4414,38 +4598,44 @@
         <v>10</v>
       </c>
       <c r="H29" s="60">
+        <v>0</v>
+      </c>
+      <c r="I29" s="60">
         <v>0.01</v>
       </c>
-      <c r="I29" s="61">
+      <c r="J29" s="61">
         <v>0.01</v>
       </c>
-      <c r="J29" s="61">
-        <v>1</v>
-      </c>
-      <c r="K29" s="61" t="s">
+      <c r="K29" s="61">
+        <v>1</v>
+      </c>
+      <c r="L29" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="L29" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M29" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N29" s="62">
-        <v>1</v>
-      </c>
-      <c r="O29" s="61">
+      <c r="M29" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="N29" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="O29" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="P29" s="62">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="61">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P29" s="84">
+      <c r="R29" s="84">
         <v>0.1</v>
       </c>
-      <c r="Q29" s="11" t="s">
+      <c r="S29" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="15" customFormat="1">
       <c r="A30" s="89">
         <v>29</v>
       </c>
@@ -4455,7 +4645,7 @@
       <c r="C30" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="63" t="s">
         <v>110</v>
       </c>
       <c r="E30" s="63" t="s">
@@ -4468,38 +4658,44 @@
         <v>10</v>
       </c>
       <c r="H30" s="65">
+        <v>0</v>
+      </c>
+      <c r="I30" s="65">
         <v>0.01</v>
       </c>
-      <c r="I30" s="66">
+      <c r="J30" s="66">
         <v>0.01</v>
       </c>
-      <c r="J30" s="66">
-        <v>1</v>
-      </c>
-      <c r="K30" s="66" t="s">
+      <c r="K30" s="66">
+        <v>1</v>
+      </c>
+      <c r="L30" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M30" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N30" s="67">
-        <v>1</v>
-      </c>
-      <c r="O30" s="66">
+      <c r="M30" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="N30" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="O30" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="P30" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="66">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P30" s="85">
+      <c r="R30" s="85">
         <v>0.1</v>
       </c>
-      <c r="Q30" s="11" t="s">
+      <c r="S30" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" s="15" customFormat="1">
       <c r="A31" s="89">
         <v>30</v>
       </c>
@@ -4509,7 +4705,7 @@
       <c r="C31" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="63" t="s">
         <v>110</v>
       </c>
       <c r="E31" s="63" t="s">
@@ -4522,38 +4718,44 @@
         <v>10</v>
       </c>
       <c r="H31" s="65">
+        <v>0</v>
+      </c>
+      <c r="I31" s="65">
         <v>0.01</v>
       </c>
-      <c r="I31" s="66">
+      <c r="J31" s="66">
         <v>0.01</v>
       </c>
-      <c r="J31" s="66">
-        <v>1</v>
-      </c>
-      <c r="K31" s="66" t="s">
+      <c r="K31" s="66">
+        <v>1</v>
+      </c>
+      <c r="L31" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="L31" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M31" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N31" s="67">
-        <v>1</v>
-      </c>
-      <c r="O31" s="66">
+      <c r="M31" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="N31" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="O31" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="P31" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="66">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P31" s="85">
+      <c r="R31" s="85">
         <v>0.1</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="S31" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" s="15" customFormat="1">
       <c r="A32" s="89">
         <v>31</v>
       </c>
@@ -4563,7 +4765,7 @@
       <c r="C32" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="68" t="s">
         <v>110</v>
       </c>
       <c r="E32" s="68" t="s">
@@ -4576,39 +4778,45 @@
         <v>10</v>
       </c>
       <c r="H32" s="70">
+        <v>0</v>
+      </c>
+      <c r="I32" s="70">
         <v>0.01</v>
       </c>
-      <c r="I32" s="71">
+      <c r="J32" s="71">
         <v>0.01</v>
       </c>
-      <c r="J32" s="71">
-        <v>1</v>
-      </c>
-      <c r="K32" s="71" t="s">
+      <c r="K32" s="71">
+        <v>1</v>
+      </c>
+      <c r="L32" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="L32" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="M32" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="N32" s="72">
-        <v>1</v>
-      </c>
-      <c r="O32" s="71">
+      <c r="M32" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="N32" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="O32" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="P32" s="72">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="71">
         <f t="shared" si="4"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P32" s="86">
+      <c r="R32" s="86">
         <v>0.1</v>
       </c>
-      <c r="Q32" s="11" t="s">
+      <c r="S32" s="11" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B5:P68">
+  <sortState ref="B5:R68">
     <sortCondition ref="B133:B196"/>
     <sortCondition ref="C133:C196"/>
   </sortState>
@@ -4618,8 +4826,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:C29"/>
@@ -4628,16 +4836,16 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="89.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="44.625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="3"/>
+    <col min="4" max="4" width="44.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="26" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -4648,7 +4856,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="15" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>71</v>
       </c>
@@ -4659,7 +4867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="15" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>71</v>
       </c>
@@ -4670,7 +4878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="15" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>71</v>
       </c>
@@ -4681,7 +4889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="15" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -4692,7 +4900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="15" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>72</v>
       </c>
@@ -4703,7 +4911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="15" customFormat="1" ht="28">
       <c r="A7" s="7" t="s">
         <v>72</v>
       </c>
@@ -4714,7 +4922,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="15" customFormat="1" ht="28">
       <c r="A8" s="7" t="s">
         <v>72</v>
       </c>
@@ -4725,7 +4933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="15" customFormat="1">
       <c r="A9" s="9" t="s">
         <v>72</v>
       </c>
@@ -4736,7 +4944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="16" customFormat="1" ht="28">
       <c r="A10" s="7" t="s">
         <v>74</v>
       </c>
@@ -4747,7 +4955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="15" customFormat="1" ht="42">
       <c r="A11" s="7" t="s">
         <v>74</v>
       </c>
@@ -4758,7 +4966,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="15" customFormat="1" ht="56">
       <c r="A12" s="7" t="s">
         <v>74</v>
       </c>
@@ -4769,7 +4977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="15" customFormat="1" ht="42">
       <c r="A13" s="7" t="s">
         <v>74</v>
       </c>
@@ -4780,7 +4988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="16" customFormat="1" ht="28">
       <c r="A14" s="7" t="s">
         <v>79</v>
       </c>
@@ -4791,7 +4999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="15" customFormat="1" ht="42">
       <c r="A15" s="7" t="s">
         <v>79</v>
       </c>
@@ -4802,7 +5010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="15" customFormat="1" ht="56">
       <c r="A16" s="7" t="s">
         <v>79</v>
       </c>
@@ -4813,7 +5021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="15" customFormat="1" ht="42">
       <c r="A17" s="7" t="s">
         <v>79</v>
       </c>
@@ -4824,7 +5032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="15" customFormat="1" ht="28">
       <c r="A18" s="8" t="s">
         <v>73</v>
       </c>
@@ -4835,7 +5043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="15" customFormat="1" ht="42">
       <c r="A19" s="7" t="s">
         <v>73</v>
       </c>
@@ -4846,7 +5054,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="15" customFormat="1" ht="56">
       <c r="A20" s="7" t="s">
         <v>73</v>
       </c>
@@ -4857,7 +5065,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="15" customFormat="1" ht="28">
       <c r="A21" s="9" t="s">
         <v>73</v>
       </c>
@@ -4868,7 +5076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="15" customFormat="1">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -4879,7 +5087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="15" customFormat="1">
       <c r="A23" s="63" t="s">
         <v>10</v>
       </c>
@@ -4890,7 +5098,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="15" customFormat="1">
       <c r="A24" s="63" t="s">
         <v>10</v>
       </c>
@@ -4901,7 +5109,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="15" customFormat="1">
       <c r="A25" s="68" t="s">
         <v>10</v>
       </c>
@@ -4912,7 +5120,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="15" customFormat="1">
       <c r="A26" s="58" t="s">
         <v>50</v>
       </c>
@@ -4923,7 +5131,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="15" customFormat="1">
       <c r="A27" s="63" t="s">
         <v>50</v>
       </c>
@@ -4934,7 +5142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="15" customFormat="1">
       <c r="A28" s="63" t="s">
         <v>50</v>
       </c>
@@ -4945,7 +5153,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="15" customFormat="1">
       <c r="A29" s="68" t="s">
         <v>50</v>
       </c>

</xml_diff>